<commit_message>
added metric definition sheet to the excel report template
</commit_message>
<xml_diff>
--- a/app/quixote-report-template.xlsx
+++ b/app/quixote-report-template.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgelouis/Desktop/quixote-app/backend/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7060567E-AC07-3645-8E2E-48949E1BE832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8CFAB7-2617-9B4C-B8B6-32CCA59874A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3140" yWindow="4220" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{5437CAEE-626D-5D4C-B5A2-31B29F604B27}"/>
+    <workbookView xWindow="3140" yWindow="4220" windowWidth="27640" windowHeight="16940" xr2:uid="{5437CAEE-626D-5D4C-B5A2-31B29F604B27}"/>
   </bookViews>
   <sheets>
-    <sheet name="summary" sheetId="5" r:id="rId1"/>
-    <sheet name="overview" sheetId="4" r:id="rId2"/>
-    <sheet name="raw-data-tracking" sheetId="1" r:id="rId3"/>
+    <sheet name="metrics-definition" sheetId="6" r:id="rId1"/>
+    <sheet name="summary" sheetId="5" r:id="rId2"/>
+    <sheet name="overview" sheetId="4" r:id="rId3"/>
+    <sheet name="raw-data-tracking" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="51" r:id="rId4"/>
+    <pivotCache cacheId="26" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>distribution_id</t>
   </si>
@@ -110,13 +111,31 @@
   </si>
   <si>
     <t>demoemail@domain.com</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>A click value of 1 (True) will be set per recipient if they have clicked on at least one of the links within a specific newsletter distribution</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>An Open value of 1 (True) will be set per recipient if they have opened the newsletter distribution at least once</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -132,8 +151,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,8 +185,20 @@
         <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -237,11 +282,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -260,6 +320,14 @@
       <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,7 +609,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="George Louis" refreshedDate="45797.044996296296" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BFA84E64-4304-0848-81E3-85F45119B26E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="George Louis" refreshedDate="45842.102248958334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="1" xr:uid="{BFA84E64-4304-0848-81E3-85F45119B26E}">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -613,7 +681,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09926FE5-DC01-B14A-9215-94D7EB64A340}" name="PivotTable4" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{09926FE5-DC01-B14A-9215-94D7EB64A340}" name="PivotTable4" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -700,7 +768,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DA9460A-6D68-D441-955E-41595528D152}" name="PivotTable5" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0DA9460A-6D68-D441-955E-41595528D152}" name="PivotTable5" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H4:M6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisPage" showAll="0">
@@ -784,7 +852,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1AC62656-744F-4D41-A858-93AC9D612679}" name="PivotTable3" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1AC62656-744F-4D41-A858-93AC9D612679}" name="PivotTable3" cacheId="26" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
@@ -1214,6 +1282,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{908C71F7-1B58-C64C-80D2-133FB8E189B5}">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="74.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="68" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5E6FE7-4077-1649-91B9-E477C6D05728}">
   <dimension ref="A1:M6"/>
   <sheetViews>
@@ -1396,11 +1507,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED0F257-6ACB-D34D-8F64-DF9D6BB07535}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -1526,7 +1637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDE6BFE-13E2-AA48-9A46-2076F16978C7}">
   <dimension ref="A1:J2"/>
   <sheetViews>

</xml_diff>